<commit_message>
README updated with usage instructions
</commit_message>
<xml_diff>
--- a/analysedStock.xlsx
+++ b/analysedStock.xlsx
@@ -510,69 +510,69 @@
     </row>
     <row r="2">
       <c r="A2" s="1" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>A</t>
+          <t>C</t>
         </is>
       </c>
       <c r="C2" t="inlineStr"/>
       <c r="D2" t="inlineStr"/>
       <c r="E2" t="n">
+        <v>3</v>
+      </c>
+      <c r="F2" t="n">
+        <v>3</v>
+      </c>
+      <c r="G2" t="inlineStr"/>
+      <c r="H2" t="n">
+        <v>4</v>
+      </c>
+      <c r="I2" t="n">
+        <v>3</v>
+      </c>
+      <c r="J2" t="n">
+        <v>6</v>
+      </c>
+      <c r="K2" t="n">
+        <v>6</v>
+      </c>
+      <c r="L2" t="n">
         <v>7</v>
       </c>
-      <c r="F2" t="n">
-        <v>2</v>
-      </c>
-      <c r="G2" t="n">
-        <v>12</v>
-      </c>
-      <c r="H2" t="n">
-        <v>6</v>
-      </c>
-      <c r="I2" t="n">
-        <v>8</v>
-      </c>
-      <c r="J2" t="n">
-        <v>7</v>
-      </c>
-      <c r="K2" t="n">
-        <v>8</v>
-      </c>
-      <c r="L2" t="n">
-        <v>5</v>
-      </c>
       <c r="M2" t="n">
-        <v>111</v>
+        <v>0</v>
       </c>
       <c r="N2" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="O2" t="n">
-        <v>13.7</v>
+        <v>0</v>
       </c>
       <c r="P2" t="n">
-        <v>5.620689655172414</v>
+        <v>10</v>
       </c>
       <c r="Q2" t="n">
-        <v>1.43</v>
+        <v>0</v>
       </c>
       <c r="R2" t="inlineStr"/>
       <c r="S2" t="n">
-        <v>19.591</v>
+        <v>0</v>
       </c>
       <c r="T2" t="inlineStr"/>
       <c r="U2" t="n">
-        <v>0.54</v>
+        <v>0</v>
       </c>
       <c r="V2" t="inlineStr"/>
       <c r="W2" t="n">
-        <v>0.33</v>
-      </c>
-      <c r="X2" t="inlineStr"/>
+        <v>0</v>
+      </c>
+      <c r="X2" t="n">
+        <v>10</v>
+      </c>
       <c r="Y2" t="n">
-        <v>33.10344827586206</v>
+        <v>1110</v>
       </c>
       <c r="Z2" t="inlineStr"/>
       <c r="AA2" t="inlineStr"/>
@@ -581,67 +581,71 @@
     </row>
     <row r="3">
       <c r="A3" s="1" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>Aurobindo pharma</t>
+          <t>A</t>
         </is>
       </c>
       <c r="C3" t="inlineStr"/>
       <c r="D3" t="inlineStr"/>
       <c r="E3" t="n">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="F3" t="n">
+        <v>2</v>
+      </c>
+      <c r="G3" t="n">
+        <v>12</v>
+      </c>
+      <c r="H3" t="n">
+        <v>6</v>
+      </c>
+      <c r="I3" t="n">
+        <v>8</v>
+      </c>
+      <c r="J3" t="n">
+        <v>7</v>
+      </c>
+      <c r="K3" t="n">
+        <v>8</v>
+      </c>
+      <c r="L3" t="n">
+        <v>5</v>
+      </c>
+      <c r="M3" t="n">
+        <v>111</v>
+      </c>
+      <c r="N3" t="n">
         <v>1</v>
       </c>
-      <c r="G3" t="inlineStr"/>
-      <c r="H3" t="n">
-        <v>4</v>
-      </c>
-      <c r="I3" t="n">
-        <v>7.5</v>
-      </c>
-      <c r="J3" t="n">
-        <v>7.5</v>
-      </c>
-      <c r="K3" t="n">
-        <v>7.5</v>
-      </c>
-      <c r="L3" t="n">
-        <v>7.5</v>
-      </c>
-      <c r="M3" t="n">
-        <v>13</v>
-      </c>
-      <c r="N3" t="n">
-        <v>9.666666666666666</v>
-      </c>
       <c r="O3" t="n">
-        <v>9.01</v>
+        <v>13.7</v>
       </c>
       <c r="P3" t="n">
-        <v>7.237931034482759</v>
+        <v>5.620689655172414</v>
       </c>
       <c r="Q3" t="n">
-        <v>1.53</v>
+        <v>1.43</v>
       </c>
       <c r="R3" t="inlineStr"/>
       <c r="S3" t="n">
-        <v>13.7853</v>
+        <v>19.591</v>
       </c>
       <c r="T3" t="inlineStr"/>
       <c r="U3" t="n">
-        <v>1.35</v>
+        <v>0.54</v>
       </c>
       <c r="V3" t="inlineStr"/>
       <c r="W3" t="n">
-        <v>0.39</v>
-      </c>
-      <c r="X3" t="inlineStr"/>
+        <v>0.33</v>
+      </c>
+      <c r="X3" t="n">
+        <v>7.444444444444444</v>
+      </c>
       <c r="Y3" t="n">
-        <v>84.52298850574712</v>
+        <v>783.1685823754789</v>
       </c>
       <c r="Z3" t="inlineStr"/>
       <c r="AA3" t="inlineStr"/>
@@ -650,67 +654,69 @@
     </row>
     <row r="4">
       <c r="A4" s="1" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>B</t>
+          <t>Aurobindo pharma</t>
         </is>
       </c>
       <c r="C4" t="inlineStr"/>
       <c r="D4" t="inlineStr"/>
       <c r="E4" t="n">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="F4" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="G4" t="inlineStr"/>
       <c r="H4" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="I4" t="n">
-        <v>4</v>
+        <v>7.5</v>
       </c>
       <c r="J4" t="n">
-        <v>3.5</v>
+        <v>7.5</v>
       </c>
       <c r="K4" t="n">
-        <v>9</v>
+        <v>7.5</v>
       </c>
       <c r="L4" t="n">
-        <v>8</v>
+        <v>7.5</v>
       </c>
       <c r="M4" t="n">
-        <v>0</v>
+        <v>13</v>
       </c>
       <c r="N4" t="n">
-        <v>10</v>
+        <v>9.666666666666666</v>
       </c>
       <c r="O4" t="n">
-        <v>22</v>
+        <v>9.01</v>
       </c>
       <c r="P4" t="n">
-        <v>2.758620689655173</v>
+        <v>7.237931034482759</v>
       </c>
       <c r="Q4" t="n">
-        <v>4.53</v>
+        <v>1.53</v>
       </c>
       <c r="R4" t="inlineStr"/>
       <c r="S4" t="n">
-        <v>99.66</v>
+        <v>13.7853</v>
       </c>
       <c r="T4" t="inlineStr"/>
       <c r="U4" t="n">
-        <v>1.72</v>
+        <v>1.35</v>
       </c>
       <c r="V4" t="inlineStr"/>
       <c r="W4" t="n">
-        <v>0.72</v>
-      </c>
-      <c r="X4" t="inlineStr"/>
+        <v>0.39</v>
+      </c>
+      <c r="X4" t="n">
+        <v>6.777777777777777</v>
+      </c>
       <c r="Y4" t="n">
-        <v>63.79310344827586</v>
+        <v>769.5386973180076</v>
       </c>
       <c r="Z4" t="inlineStr"/>
       <c r="AA4" t="inlineStr"/>
@@ -719,36 +725,36 @@
     </row>
     <row r="5">
       <c r="A5" s="1" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>C</t>
+          <t>B</t>
         </is>
       </c>
       <c r="C5" t="inlineStr"/>
       <c r="D5" t="inlineStr"/>
       <c r="E5" t="n">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="F5" t="n">
         <v>3</v>
       </c>
       <c r="G5" t="inlineStr"/>
       <c r="H5" t="n">
+        <v>3</v>
+      </c>
+      <c r="I5" t="n">
         <v>4</v>
       </c>
-      <c r="I5" t="n">
-        <v>3</v>
-      </c>
       <c r="J5" t="n">
-        <v>6</v>
+        <v>3.5</v>
       </c>
       <c r="K5" t="n">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="L5" t="n">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="M5" t="n">
         <v>0</v>
@@ -757,29 +763,31 @@
         <v>10</v>
       </c>
       <c r="O5" t="n">
-        <v>0</v>
+        <v>22</v>
       </c>
       <c r="P5" t="n">
-        <v>10</v>
+        <v>2.758620689655173</v>
       </c>
       <c r="Q5" t="n">
-        <v>0</v>
+        <v>4.53</v>
       </c>
       <c r="R5" t="inlineStr"/>
       <c r="S5" t="n">
-        <v>0</v>
+        <v>99.66</v>
       </c>
       <c r="T5" t="inlineStr"/>
       <c r="U5" t="n">
-        <v>0</v>
+        <v>1.72</v>
       </c>
       <c r="V5" t="inlineStr"/>
       <c r="W5" t="n">
-        <v>0</v>
-      </c>
-      <c r="X5" t="inlineStr"/>
+        <v>0.72</v>
+      </c>
+      <c r="X5" t="n">
+        <v>3.111111111111111</v>
+      </c>
       <c r="Y5" t="n">
-        <v>100</v>
+        <v>377.6628352490422</v>
       </c>
       <c r="Z5" t="inlineStr"/>
       <c r="AA5" t="inlineStr"/>
@@ -846,9 +854,11 @@
       <c r="W6" t="n">
         <v>1.7</v>
       </c>
-      <c r="X6" t="inlineStr"/>
+      <c r="X6" t="n">
+        <v>1</v>
+      </c>
       <c r="Y6" t="n">
-        <v>10</v>
+        <v>111</v>
       </c>
       <c r="Z6" t="inlineStr"/>
       <c r="AA6" t="inlineStr"/>

</xml_diff>